<commit_message>
use data MarketPull and Push
</commit_message>
<xml_diff>
--- a/data-raw/varsList.xlsx
+++ b/data-raw/varsList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\techme\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D46A21-A72B-4B69-834E-DF603E61FB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A464E49-3C91-4715-8CBE-31546A85D657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3195" yWindow="8002" windowWidth="24495" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -5966,8 +5966,8 @@
   <dimension ref="A1:P489"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E364" sqref="E364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19556,8 +19556,8 @@
       <c r="D361" t="s">
         <v>1499</v>
       </c>
-      <c r="E361" t="s">
-        <v>525</v>
+      <c r="E361" s="1" t="s">
+        <v>1243</v>
       </c>
       <c r="F361" t="s">
         <v>808</v>
@@ -19632,8 +19632,8 @@
       <c r="D363" t="s">
         <v>1501</v>
       </c>
-      <c r="E363" t="s">
-        <v>525</v>
+      <c r="E363" s="1" t="s">
+        <v>1243</v>
       </c>
       <c r="F363" t="s">
         <v>808</v>

</xml_diff>

<commit_message>
obs station most 2019
</commit_message>
<xml_diff>
--- a/data-raw/varsList.xlsx
+++ b/data-raw/varsList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\techme\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F9C550-F324-4BAE-B4EE-EAF3379875A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17226621-09DE-43BA-9018-5E35DEF1D698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3090" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6936" uniqueCount="1709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7152" uniqueCount="1719">
   <si>
     <t>variables</t>
   </si>
@@ -5997,15 +5997,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>v2022.8</t>
-  </si>
-  <si>
-    <t>v2022.9</t>
-  </si>
-  <si>
-    <t>v2022.10</t>
-  </si>
-  <si>
     <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6023,6 +6014,57 @@
   </si>
   <si>
     <t>公共网站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>agripark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国家农业科技园区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v2022.7</t>
+  </si>
+  <si>
+    <t>batch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>评估</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验收</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6497,11 +6539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P596"/>
+  <dimension ref="A1:P611"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A578" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I593" sqref="I593"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H598" sqref="H598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29419,7 +29461,7 @@
     </row>
     <row r="588" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A588" t="str">
-        <f t="shared" ref="A588:A593" si="11">F588&amp;"_"&amp;G588&amp;"_"&amp;H588&amp;"_"&amp;I588</f>
+        <f t="shared" ref="A588:A600" si="11">F588&amp;"_"&amp;G588&amp;"_"&amp;H588&amp;"_"&amp;I588</f>
         <v>v99_obstation_list_index</v>
       </c>
       <c r="C588" s="1" t="s">
@@ -29432,7 +29474,7 @@
         <v>1686</v>
       </c>
       <c r="G588" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="H588" t="s">
         <v>1687</v>
@@ -29441,7 +29483,7 @@
         <v>1691</v>
       </c>
       <c r="J588" s="1" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="K588" s="1" t="s">
         <v>1688</v>
@@ -29465,7 +29507,7 @@
         <v>v99_obstation_list_name</v>
       </c>
       <c r="C589" s="1" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="D589" t="s">
         <v>1692</v>
@@ -29474,7 +29516,7 @@
         <v>1686</v>
       </c>
       <c r="G589" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="H589" t="s">
         <v>1687</v>
@@ -29483,7 +29525,7 @@
         <v>1692</v>
       </c>
       <c r="J589" s="1" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="K589" s="1" t="s">
         <v>1688</v>
@@ -29516,7 +29558,7 @@
         <v>1685</v>
       </c>
       <c r="G590" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="H590" t="s">
         <v>1687</v>
@@ -29525,7 +29567,7 @@
         <v>1525</v>
       </c>
       <c r="J590" s="1" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="K590" s="1" t="s">
         <v>1688</v>
@@ -29537,7 +29579,7 @@
         <v>1696</v>
       </c>
       <c r="O590" t="s">
-        <v>1701</v>
+        <v>1708</v>
       </c>
       <c r="P590" s="1" t="s">
         <v>1700</v>
@@ -29558,7 +29600,7 @@
         <v>1685</v>
       </c>
       <c r="G591" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="H591" t="s">
         <v>1687</v>
@@ -29567,7 +29609,7 @@
         <v>1693</v>
       </c>
       <c r="J591" s="1" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="K591" s="1" t="s">
         <v>1688</v>
@@ -29579,7 +29621,7 @@
         <v>1697</v>
       </c>
       <c r="O591" t="s">
-        <v>1702</v>
+        <v>1708</v>
       </c>
       <c r="P591" s="1" t="s">
         <v>1700</v>
@@ -29591,25 +29633,25 @@
         <v>v99_obstation_list_officer</v>
       </c>
       <c r="C592" s="1" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="D592" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F592" t="s">
         <v>1685</v>
       </c>
       <c r="G592" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="H592" t="s">
         <v>1687</v>
       </c>
       <c r="I592" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="J592" s="1" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="K592" s="1" t="s">
         <v>1688</v>
@@ -29618,10 +29660,10 @@
         <v>1689</v>
       </c>
       <c r="M592" s="1" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="O592" t="s">
-        <v>1703</v>
+        <v>1708</v>
       </c>
       <c r="P592" s="1" t="s">
         <v>1700</v>
@@ -29642,7 +29684,7 @@
         <v>1685</v>
       </c>
       <c r="G593" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="H593" t="s">
         <v>1687</v>
@@ -29651,7 +29693,7 @@
         <v>1694</v>
       </c>
       <c r="J593" s="1" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="K593" s="1" t="s">
         <v>1688</v>
@@ -29663,23 +29705,767 @@
         <v>1698</v>
       </c>
       <c r="O593" t="s">
-        <v>1703</v>
+        <v>1708</v>
       </c>
       <c r="P593" s="1" t="s">
         <v>1700</v>
       </c>
     </row>
     <row r="594" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K594" s="1"/>
-      <c r="L594" s="1"/>
+      <c r="A594" t="str">
+        <f t="shared" ref="A594" si="12">F594&amp;"_"&amp;G594&amp;"_"&amp;H594&amp;"_"&amp;I594</f>
+        <v>v99_agripark_list_year</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D594" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F594" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G594" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H594" t="s">
+        <v>1687</v>
+      </c>
+      <c r="I594" t="s">
+        <v>1712</v>
+      </c>
+      <c r="J594" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K594" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L594" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="M594" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="O594" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P594" s="1" t="s">
+        <v>1700</v>
+      </c>
     </row>
     <row r="595" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K595" s="1"/>
-      <c r="L595" s="1"/>
+      <c r="A595" t="str">
+        <f t="shared" si="11"/>
+        <v>v99_agripark_list_index</v>
+      </c>
+      <c r="C595" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D595" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F595" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G595" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H595" t="s">
+        <v>1687</v>
+      </c>
+      <c r="I595" t="s">
+        <v>1691</v>
+      </c>
+      <c r="J595" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K595" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L595" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="M595" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="O595" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P595" s="1" t="s">
+        <v>1700</v>
+      </c>
     </row>
     <row r="596" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K596" s="1"/>
-      <c r="L596" s="1"/>
+      <c r="A596" t="str">
+        <f t="shared" si="11"/>
+        <v>v99_agripark_list_batch</v>
+      </c>
+      <c r="C596" s="1" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D596" t="s">
+        <v>1709</v>
+      </c>
+      <c r="F596" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G596" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H596" t="s">
+        <v>1687</v>
+      </c>
+      <c r="I596" t="s">
+        <v>1709</v>
+      </c>
+      <c r="J596" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K596" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L596" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="M596" s="1" t="s">
+        <v>1710</v>
+      </c>
+      <c r="O596" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P596" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="597" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A597" t="str">
+        <f t="shared" si="11"/>
+        <v>v99_agripark_list_name</v>
+      </c>
+      <c r="C597" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D597" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F597" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G597" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H597" t="s">
+        <v>1687</v>
+      </c>
+      <c r="I597" t="s">
+        <v>1692</v>
+      </c>
+      <c r="J597" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K597" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L597" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="M597" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="O597" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P597" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="598" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A598" t="str">
+        <f t="shared" si="11"/>
+        <v>v99_agripark_list_province</v>
+      </c>
+      <c r="C598" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D598" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F598" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G598" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H598" t="s">
+        <v>1687</v>
+      </c>
+      <c r="I598" t="s">
+        <v>1694</v>
+      </c>
+      <c r="J598" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K598" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L598" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="M598" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="O598" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P598" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="599" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A599" t="str">
+        <f t="shared" si="11"/>
+        <v>v99_agripark_list_officer</v>
+      </c>
+      <c r="C599" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D599" t="s">
+        <v>1703</v>
+      </c>
+      <c r="F599" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G599" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H599" t="s">
+        <v>1687</v>
+      </c>
+      <c r="I599" t="s">
+        <v>1703</v>
+      </c>
+      <c r="J599" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K599" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L599" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="M599" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="O599" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P599" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="600" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A600" t="str">
+        <f t="shared" si="11"/>
+        <v>v99_agripark_eval_year</v>
+      </c>
+      <c r="C600" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D600" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F600" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G600" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H600" t="s">
+        <v>1713</v>
+      </c>
+      <c r="I600" t="s">
+        <v>1712</v>
+      </c>
+      <c r="J600" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K600" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L600" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="M600" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="O600" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P600" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="601" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A601" t="str">
+        <f t="shared" ref="A601:A606" si="13">F601&amp;"_"&amp;G601&amp;"_"&amp;H601&amp;"_"&amp;I601</f>
+        <v>v99_agripark_eval_index</v>
+      </c>
+      <c r="C601" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D601" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F601" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G601" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H601" t="s">
+        <v>1713</v>
+      </c>
+      <c r="I601" t="s">
+        <v>1691</v>
+      </c>
+      <c r="J601" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K601" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L601" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="M601" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="O601" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P601" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="602" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A602" t="str">
+        <f t="shared" si="13"/>
+        <v>v99_agripark_eval_name</v>
+      </c>
+      <c r="C602" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D602" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F602" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G602" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H602" t="s">
+        <v>1713</v>
+      </c>
+      <c r="I602" t="s">
+        <v>1692</v>
+      </c>
+      <c r="J602" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K602" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L602" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="M602" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="O602" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P602" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="603" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A603" t="str">
+        <f t="shared" ref="A603" si="14">F603&amp;"_"&amp;G603&amp;"_"&amp;H603&amp;"_"&amp;I603</f>
+        <v>v99_agripark_eval_result</v>
+      </c>
+      <c r="C603" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D603" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F603" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G603" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H603" t="s">
+        <v>1713</v>
+      </c>
+      <c r="I603" t="s">
+        <v>1714</v>
+      </c>
+      <c r="J603" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K603" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L603" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="M603" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="O603" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P603" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="604" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A604" t="str">
+        <f t="shared" si="13"/>
+        <v>v99_agripark_eval_province</v>
+      </c>
+      <c r="C604" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D604" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F604" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G604" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H604" t="s">
+        <v>1713</v>
+      </c>
+      <c r="I604" t="s">
+        <v>1694</v>
+      </c>
+      <c r="J604" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K604" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L604" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="M604" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="O604" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P604" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="605" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A605" t="str">
+        <f t="shared" si="13"/>
+        <v>v99_agripark_eval_officer</v>
+      </c>
+      <c r="C605" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D605" t="s">
+        <v>1703</v>
+      </c>
+      <c r="F605" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G605" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H605" t="s">
+        <v>1713</v>
+      </c>
+      <c r="I605" t="s">
+        <v>1703</v>
+      </c>
+      <c r="J605" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K605" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L605" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="M605" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="O605" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P605" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="606" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A606" t="str">
+        <f t="shared" si="13"/>
+        <v>v99_agripark_check_year</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D606" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F606" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G606" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H606" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I606" t="s">
+        <v>1712</v>
+      </c>
+      <c r="J606" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K606" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L606" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="M606" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="O606" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P606" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="607" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A607" t="str">
+        <f t="shared" ref="A607:A611" si="15">F607&amp;"_"&amp;G607&amp;"_"&amp;H607&amp;"_"&amp;I607</f>
+        <v>v99_agripark_check_index</v>
+      </c>
+      <c r="C607" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D607" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F607" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G607" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H607" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I607" t="s">
+        <v>1691</v>
+      </c>
+      <c r="J607" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K607" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L607" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="M607" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="O607" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P607" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="608" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A608" t="str">
+        <f t="shared" si="15"/>
+        <v>v99_agripark_check_name</v>
+      </c>
+      <c r="C608" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D608" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F608" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G608" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H608" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I608" t="s">
+        <v>1692</v>
+      </c>
+      <c r="J608" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K608" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L608" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="M608" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="O608" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P608" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="609" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A609" t="str">
+        <f t="shared" si="15"/>
+        <v>v99_agripark_check_result</v>
+      </c>
+      <c r="C609" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D609" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F609" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G609" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H609" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I609" t="s">
+        <v>1714</v>
+      </c>
+      <c r="J609" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K609" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L609" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="M609" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="O609" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P609" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="610" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A610" t="str">
+        <f t="shared" si="15"/>
+        <v>v99_agripark_check_province</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D610" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F610" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G610" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H610" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I610" t="s">
+        <v>1694</v>
+      </c>
+      <c r="J610" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K610" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L610" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="M610" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="O610" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P610" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="611" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A611" t="str">
+        <f t="shared" si="15"/>
+        <v>v99_agripark_check_officer</v>
+      </c>
+      <c r="C611" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D611" t="s">
+        <v>1703</v>
+      </c>
+      <c r="F611" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G611" t="s">
+        <v>1706</v>
+      </c>
+      <c r="H611" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I611" t="s">
+        <v>1703</v>
+      </c>
+      <c r="J611" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K611" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="L611" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="M611" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="O611" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P611" s="1" t="s">
+        <v>1700</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>